<commit_message>
view-extension.js for pdf view. + dynamic word selection
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -387,22 +387,12 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>nd algori</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>ibonacci</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Fibonacci</v>
+        <v>（我这里用的是【3.11.174】版本</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>